<commit_message>
Add a new oligo panel
Closes #111
</commit_message>
<xml_diff>
--- a/cosmx-transcriptomics/latest/cosmx-transcriptomics.xlsx
+++ b/cosmx-transcriptomics/latest/cosmx-transcriptomics.xlsx
@@ -257,7 +257,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="442">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -277,48 +277,168 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000195</t>
   </si>
   <si>
+    <t>SNARE-seq2</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000264</t>
+  </si>
+  <si>
+    <t>Visium (no probes)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000302</t>
+  </si>
+  <si>
+    <t>DESI</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000204</t>
+  </si>
+  <si>
+    <t>Confocal</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
+  </si>
+  <si>
+    <t>Stereo-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
+  </si>
+  <si>
+    <t>Visium (with probes)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000303</t>
+  </si>
+  <si>
+    <t>Molecular Cartography</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
+  </si>
+  <si>
+    <t>DBiT-seq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
+  </si>
+  <si>
+    <t>Seq-Scope</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000390</t>
+  </si>
+  <si>
+    <t>CosMx Transcriptomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
+  </si>
+  <si>
+    <t>CyCIF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000200</t>
+  </si>
+  <si>
+    <t>Light Sheet</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
+  </si>
+  <si>
+    <t>seqFISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000397</t>
+  </si>
+  <si>
+    <t>ATACseq</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
+  </si>
+  <si>
+    <t>CosMx Proteomics</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000435</t>
+  </si>
+  <si>
+    <t>Singular Genomics G4X</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000429</t>
+  </si>
+  <si>
+    <t>Visium HD</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000451</t>
+  </si>
+  <si>
+    <t>MERFISH</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000221</t>
+  </si>
+  <si>
+    <t>10X Multiome</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
+  </si>
+  <si>
+    <t>4i</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000447</t>
+  </si>
+  <si>
+    <t>PhenoCycler</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000199</t>
+  </si>
+  <si>
+    <t>Second Harmonic Generation (SHG)</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000208</t>
+  </si>
+  <si>
+    <t>Thick section Multiphoton MxIF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
+  </si>
+  <si>
+    <t>CyTOF</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000407</t>
+  </si>
+  <si>
     <t>Olink</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000441</t>
   </si>
   <si>
-    <t>SNARE-seq2</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000264</t>
-  </si>
-  <si>
     <t>MIBI</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000172</t>
   </si>
   <si>
-    <t>Visium (no probes)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000302</t>
-  </si>
-  <si>
-    <t>DESI</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000204</t>
-  </si>
-  <si>
     <t>Auto-fluorescence</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000205</t>
   </si>
   <si>
-    <t>Confocal</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000206</t>
-  </si>
-  <si>
     <t>FACS</t>
   </si>
   <si>
@@ -331,42 +451,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000219</t>
   </si>
   <si>
-    <t>Stereo-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000385</t>
-  </si>
-  <si>
-    <t>Visium (with probes)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000303</t>
-  </si>
-  <si>
-    <t>Molecular Cartography</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000217</t>
-  </si>
-  <si>
-    <t>CosMx</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000218</t>
-  </si>
-  <si>
-    <t>DBiT-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000428</t>
-  </si>
-  <si>
-    <t>Seq-Scope</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000390</t>
-  </si>
-  <si>
     <t>SIMS</t>
   </si>
   <si>
@@ -397,16 +481,10 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000328</t>
   </si>
   <si>
-    <t>CyCIF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000200</t>
-  </si>
-  <si>
-    <t>Light Sheet</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000168</t>
+    <t>Pixel-seqV2</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000450</t>
   </si>
   <si>
     <t>MALDI</t>
@@ -415,30 +493,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000201</t>
   </si>
   <si>
-    <t>seqFISH</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000397</t>
-  </si>
-  <si>
     <t>2D Imaging Mass Cytometry</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000296</t>
   </si>
   <si>
-    <t>ATACseq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000309</t>
-  </si>
-  <si>
-    <t>CosMx Proteomics</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000435</t>
-  </si>
-  <si>
     <t>Histology</t>
   </si>
   <si>
@@ -469,18 +529,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000310</t>
   </si>
   <si>
-    <t>Singular Genomics G4X</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000429</t>
-  </si>
-  <si>
-    <t>MERFISH</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000221</t>
-  </si>
-  <si>
     <t>LC-MS</t>
   </si>
   <si>
@@ -493,18 +541,6 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000312</t>
   </si>
   <si>
-    <t>Pixel-seq</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000449</t>
-  </si>
-  <si>
-    <t>10X Multiome</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000215</t>
-  </si>
-  <si>
     <t>GeoMx (nCounter)</t>
   </si>
   <si>
@@ -517,51 +553,18 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000311</t>
   </si>
   <si>
-    <t>4i</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000447</t>
-  </si>
-  <si>
-    <t>PhenoCycler</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000199</t>
-  </si>
-  <si>
-    <t>Second Harmonic Generation (SHG)</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000208</t>
-  </si>
-  <si>
-    <t>Thick section Multiphoton MxIF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000207</t>
-  </si>
-  <si>
     <t>MS Lipidomics</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000405</t>
   </si>
   <si>
-    <t>CyTOF</t>
-  </si>
-  <si>
-    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000407</t>
-  </si>
-  <si>
     <t>MPLEx</t>
   </si>
   <si>
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000448</t>
   </si>
   <si>
-    <t>CosMx Transcriptomics</t>
-  </si>
-  <si>
     <t>analyte_class</t>
   </si>
   <si>
@@ -1426,6 +1429,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000442</t>
   </si>
   <si>
+    <t>NanoString Technologies; CosMx Mouse Neuroscience Panel (RNA, 1000 Plex); PN CMX-M-NEUP-R</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000452</t>
+  </si>
+  <si>
     <t>10x Genomics; Visium Human Transcriptome Probe Kit-Small; PN 1000363</t>
   </si>
   <si>
@@ -1567,7 +1576,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-07-24T21:05:36-07:00</t>
+    <t>2025-08-15T09:10:02-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1727,102 +1736,102 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>430</v>
+        <v>433</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="AF2" t="s" s="33">
-        <v>431</v>
+        <v>434</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="22">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$48</formula1>
+      <formula1>'dataset_type'!$A$1:$A$49</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$16</formula1>
@@ -1887,7 +1896,7 @@
       <formula1>'probe_hybridization_time_unit'!$A$1:$A$2</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="Z2:Z1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'oligo_probe_panel'!$A$1:$A$23</formula1>
+      <formula1>'oligo_probe_panel'!$A$1:$A$24</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="AA2:AA1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'is_custom_probes_used'!$A$1:$A$2</formula1>
@@ -1913,10 +1922,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -1934,10 +1943,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -1955,18 +1964,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -1976,7 +1985,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1984,186 +1993,194 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>424</v>
+        <v>425</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>426</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -2181,12 +2198,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2210,30 +2227,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>437</v>
+        <v>440</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>438</v>
+        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -2243,7 +2260,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2631,6 +2648,14 @@
       </c>
       <c r="B48" t="s" s="0">
         <v>99</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>100</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2648,130 +2673,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2789,12 +2814,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2812,242 +2837,242 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -3065,602 +3090,602 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s" s="0">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s" s="0">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s" s="0">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s" s="0">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s" s="0">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B73" t="s" s="0">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s" s="0">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B74" t="s" s="0">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s" s="0">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B75" t="s" s="0">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -3678,42 +3703,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -3731,26 +3756,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -3768,18 +3793,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix dataset type error
</commit_message>
<xml_diff>
--- a/cosmx-transcriptomics/latest/cosmx-transcriptomics.xlsx
+++ b/cosmx-transcriptomics/latest/cosmx-transcriptomics.xlsx
@@ -219,9 +219,9 @@
     </comment>
     <comment ref="Z1" authorId="1">
       <text>
-        <t>The oligo probe panel used to target genes and/or proteins. If there is a core
-panel along with add-on modules, the core panel should be selected in this
-field. Any additional panels utilized should be documented in the
+        <t>(Required) The oligo probe panel used to target genes and/or proteins. If there
+is a core panel along with add-on modules, the core panel should be selected in
+this field. Any additional panels utilized should be documented in the
 "additional_panels_used.csv" file, which must be uploaded alongside the dataset.
 Example: 10x Genomics; Visium Human Transcriptome Probe Kit-Small; PN 1000363</t>
       </text>
@@ -288,7 +288,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="456">
   <si>
     <t>parent_sample_id</t>
   </si>
@@ -314,6 +314,12 @@
     <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000264</t>
   </si>
   <si>
+    <t>COMET</t>
+  </si>
+  <si>
+    <t>https://purl.humanatlas.io/vocab/hravs#HRAVS_0000458</t>
+  </si>
+  <si>
     <t>Visium (no probes)</t>
   </si>
   <si>
@@ -1643,7 +1649,7 @@
     <t>pav:createdOn</t>
   </si>
   <si>
-    <t>2025-10-09T11:05:17-07:00</t>
+    <t>2025-10-14T09:40:00-07:00</t>
   </si>
   <si>
     <t>pav:derivedFrom</t>
@@ -1805,105 +1811,105 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H1" t="s" s="1">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="I1" t="s" s="1">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="J1" t="s" s="1">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="K1" t="s" s="1">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="L1" t="s" s="1">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="M1" t="s" s="1">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="N1" t="s" s="1">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="O1" t="s" s="1">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="P1" t="s" s="1">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="Q1" t="s" s="1">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="R1" t="s" s="1">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="S1" t="s" s="1">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="T1" t="s" s="1">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="U1" t="s" s="1">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="V1" t="s" s="1">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="W1" t="s" s="1">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="X1" t="s" s="1">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="Y1" t="s" s="1">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="Z1" t="s" s="1">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="AA1" t="s" s="1">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="AB1" t="s" s="1">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="AC1" t="s" s="1">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="AD1" t="s" s="1">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="AE1" t="s" s="1">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="AF1" t="s" s="1">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="AG1" t="s" s="1">
-        <v>445</v>
+        <v>447</v>
       </c>
     </row>
     <row r="2">
       <c r="D2" t="s" s="5">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="AG2" t="s" s="34">
-        <v>446</v>
+        <v>448</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="22">
     <dataValidation type="list" sqref="D2:D1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
-      <formula1>'dataset_type'!$A$1:$A$49</formula1>
+      <formula1>'dataset_type'!$A$1:$A$50</formula1>
     </dataValidation>
     <dataValidation type="list" sqref="E2:E1001" allowBlank="true" errorStyle="stop" errorTitle="Validation Error" error="" showErrorMessage="true">
       <formula1>'analyte_class'!$A$1:$A$16</formula1>
@@ -1994,10 +2000,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -2015,10 +2021,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -2036,18 +2042,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -2065,226 +2071,226 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>384</v>
+        <v>386</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>388</v>
+        <v>390</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>404</v>
+        <v>406</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>406</v>
+        <v>408</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>408</v>
+        <v>410</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>410</v>
+        <v>412</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>414</v>
+        <v>416</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>418</v>
+        <v>420</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>422</v>
+        <v>424</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>430</v>
+        <v>432</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>432</v>
+        <v>434</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>438</v>
+        <v>440</v>
       </c>
     </row>
   </sheetData>
@@ -2302,12 +2308,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2331,30 +2337,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="D1" t="s" s="0">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>453</v>
+        <v>455</v>
       </c>
     </row>
   </sheetData>
@@ -2364,7 +2370,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2760,6 +2766,14 @@
       </c>
       <c r="B49" t="s" s="0">
         <v>101</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2777,130 +2791,130 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2918,12 +2932,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2941,242 +2955,242 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -3194,618 +3208,618 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="0">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="0">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="0">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s" s="0">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="0">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="0">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="0">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="0">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="0">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="0">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="0">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="0">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B58" t="s" s="0">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="0">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="0">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="0">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="0">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="0">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="0">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="0">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="0">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s" s="0">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="0">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B68" t="s" s="0">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s" s="0">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B69" t="s" s="0">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s" s="0">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B70" t="s" s="0">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s" s="0">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B71" t="s" s="0">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s" s="0">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B72" t="s" s="0">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s" s="0">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B73" t="s" s="0">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s" s="0">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B74" t="s" s="0">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s" s="0">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B75" t="s" s="0">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s" s="0">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B76" t="s" s="0">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s" s="0">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B77" t="s" s="0">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -3823,42 +3837,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -3876,26 +3890,26 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -3913,18 +3927,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>